<commit_message>
lista 01 aula 2
</commit_message>
<xml_diff>
--- a/Docs/Lista01.xlsx
+++ b/Docs/Lista01.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\curso-excel\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF0E281F-F04D-4E7B-BD1D-D4C016B08EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A270E3-9B0A-4A5B-99ED-B5B2AFEA9E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exerc1" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,25 @@
     <sheet name="Exerc3" sheetId="3" r:id="rId3"/>
     <sheet name="Exerc4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="95">
   <si>
     <t>Equação</t>
   </si>
@@ -316,11 +329,20 @@
   <si>
     <t>DVD</t>
   </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Sobrenome</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="[$R$-416]&quot; &quot;#,##0.00;[Red]&quot;-&quot;[$R$-416]&quot; &quot;#,##0.00"/>
@@ -468,7 +490,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -480,7 +502,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -499,11 +520,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Heading" xfId="1"/>
-    <cellStyle name="Heading1" xfId="2"/>
+    <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Heading1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Result" xfId="3"/>
-    <cellStyle name="Result2" xfId="4"/>
+    <cellStyle name="Result" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Result2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -570,8 +591,8 @@
   <xdr:absoluteAnchor>
     <xdr:pos x="1358615" y="224302"/>
     <xdr:ext cx="368960" cy="173918"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CaixaDeTexto 2">
@@ -639,7 +660,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CaixaDeTexto 2">
@@ -695,8 +716,8 @@
   <xdr:absoluteAnchor>
     <xdr:pos x="1348191" y="475945"/>
     <xdr:ext cx="417606" cy="195498"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CaixaDeTexto 3">
@@ -742,7 +763,7 @@
                     <m:sSub>
                       <m:sSubPr>
                         <m:ctrlPr>
-                          <a:rPr lang="pt-BR">
+                          <a:rPr lang="pt-BR" i="1">
                             <a:solidFill>
                               <a:srgbClr val="836967"/>
                             </a:solidFill>
@@ -786,7 +807,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CaixaDeTexto 3">
@@ -857,8 +878,8 @@
   <xdr:absoluteAnchor>
     <xdr:pos x="1347825" y="714603"/>
     <xdr:ext cx="367954" cy="173918"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="CaixaDeTexto 4">
@@ -926,7 +947,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="CaixaDeTexto 4">
@@ -982,8 +1003,8 @@
   <xdr:absoluteAnchor>
     <xdr:pos x="1367668" y="943935"/>
     <xdr:ext cx="194401" cy="195498"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="CaixaDeTexto 5">
@@ -1029,7 +1050,7 @@
                     <m:sSup>
                       <m:sSupPr>
                         <m:ctrlPr>
-                          <a:rPr lang="pt-BR">
+                          <a:rPr lang="pt-BR" i="1">
                             <a:solidFill>
                               <a:srgbClr val="836967"/>
                             </a:solidFill>
@@ -1064,7 +1085,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="CaixaDeTexto 5">
@@ -1135,8 +1156,8 @@
   <xdr:absoluteAnchor>
     <xdr:pos x="1118128" y="1505559"/>
     <xdr:ext cx="724296" cy="393466"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="CaixaDeTexto 6">
@@ -1182,7 +1203,7 @@
                     <m:f>
                       <m:fPr>
                         <m:ctrlPr>
-                          <a:rPr lang="pt-BR">
+                          <a:rPr lang="pt-BR" i="1">
                             <a:solidFill>
                               <a:srgbClr val="836967"/>
                             </a:solidFill>
@@ -1256,7 +1277,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="CaixaDeTexto 6">
@@ -1351,8 +1372,8 @@
   <xdr:absoluteAnchor>
     <xdr:pos x="1276959" y="1210665"/>
     <xdr:ext cx="394197" cy="187177"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="CaixaDeTexto 7">
@@ -1399,7 +1420,7 @@
                       <m:radPr>
                         <m:degHide m:val="on"/>
                         <m:ctrlPr>
-                          <a:rPr lang="pt-BR">
+                          <a:rPr lang="pt-BR" i="1">
                             <a:solidFill>
                               <a:srgbClr val="836967"/>
                             </a:solidFill>
@@ -1427,7 +1448,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="CaixaDeTexto 7">
@@ -1492,8 +1513,8 @@
   <xdr:absoluteAnchor>
     <xdr:pos x="1347825" y="1962759"/>
     <xdr:ext cx="226039" cy="173918"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CaixaDeTexto 8">
@@ -1558,7 +1579,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CaixaDeTexto 8">
@@ -1614,8 +1635,8 @@
   <xdr:absoluteAnchor>
     <xdr:pos x="1168237" y="2211476"/>
     <xdr:ext cx="742675" cy="175290"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="CaixaDeTexto 9">
@@ -1691,7 +1712,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="CaixaDeTexto 9">
@@ -1747,8 +1768,8 @@
   <xdr:absoluteAnchor>
     <xdr:pos x="1119225" y="2490094"/>
     <xdr:ext cx="866119" cy="420806"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="CaixaDeTexto 10">
@@ -1794,7 +1815,7 @@
                     <m:f>
                       <m:fPr>
                         <m:ctrlPr>
-                          <a:rPr lang="pt-BR">
+                          <a:rPr lang="pt-BR" i="1">
                             <a:solidFill>
                               <a:srgbClr val="836967"/>
                             </a:solidFill>
@@ -1944,7 +1965,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="CaixaDeTexto 10">
@@ -2069,8 +2090,8 @@
   <xdr:absoluteAnchor>
     <xdr:pos x="1058052" y="3036630"/>
     <xdr:ext cx="1081095" cy="398861"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="CaixaDeTexto 11">
@@ -2116,7 +2137,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="pt-BR">
+                          <a:rPr lang="pt-BR" i="1">
                             <a:solidFill>
                               <a:srgbClr val="836967"/>
                             </a:solidFill>
@@ -2137,7 +2158,7 @@
                               </m:mc>
                             </m:mcs>
                             <m:ctrlPr>
-                              <a:rPr lang="pt-BR">
+                              <a:rPr lang="pt-BR" i="1">
                                 <a:solidFill>
                                   <a:srgbClr val="836967"/>
                                 </a:solidFill>
@@ -2235,7 +2256,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="CaixaDeTexto 11">
@@ -2631,18 +2652,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.3984375" customWidth="1"/>
-    <col min="2" max="2" width="26.8984375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="55.19921875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="26.8984375" customWidth="1"/>
+    <col min="3" max="3" width="55.19921875" customWidth="1"/>
     <col min="4" max="1024" width="8.3984375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2743,7 +2764,7 @@
       <c r="C13" s="4"/>
     </row>
     <row r="16" spans="1:3" ht="12.75" customHeight="1">
-      <c r="C16" s="8"/>
+      <c r="C16" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.78739999999999999" right="0.78739999999999999" top="1.2792000000000001" bottom="1.2792000000000001" header="0.9839" footer="0.9839"/>
@@ -2754,10 +2775,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1"/>
   <cols>
@@ -2765,91 +2788,102 @@
     <col min="2" max="2" width="32.19921875" customWidth="1"/>
     <col min="3" max="3" width="33.59765625" customWidth="1"/>
     <col min="4" max="4" width="42.09765625" customWidth="1"/>
-    <col min="5" max="1024" width="8.3984375" customWidth="1"/>
+    <col min="5" max="5" width="25.296875" customWidth="1"/>
+    <col min="6" max="6" width="23.19921875" customWidth="1"/>
+    <col min="7" max="1024" width="8.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="12.75" customHeight="1">
+      <c r="D1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="12.75" customHeight="1">
       <c r="A2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="12.75" customHeight="1">
+    <row r="3" spans="1:6" ht="12.75" customHeight="1">
       <c r="A3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="12.75" customHeight="1">
+    <row r="4" spans="1:6" ht="12.75" customHeight="1">
       <c r="A4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="12.75" customHeight="1">
+    <row r="5" spans="1:6" ht="12.75" customHeight="1">
       <c r="A5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="12.75" customHeight="1">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1">
       <c r="A6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="12.75" customHeight="1">
+    <row r="7" spans="1:6" ht="12.75" customHeight="1">
       <c r="A7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="12.75" customHeight="1">
+    <row r="8" spans="1:6" ht="12.75" customHeight="1">
       <c r="A8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="12.75" customHeight="1">
+    <row r="9" spans="1:6" ht="12.75" customHeight="1">
       <c r="A9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="12.75" customHeight="1">
+    <row r="10" spans="1:6" ht="12.75" customHeight="1">
       <c r="A10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="12.75" customHeight="1">
+    <row r="11" spans="1:6" ht="12.75" customHeight="1">
       <c r="A11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="12.75" customHeight="1">
+    <row r="12" spans="1:6" ht="12.75" customHeight="1">
       <c r="A12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="12.75" customHeight="1">
+    <row r="13" spans="1:6" ht="12.75" customHeight="1">
       <c r="A13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="12.75" customHeight="1">
+    <row r="14" spans="1:6" ht="12.75" customHeight="1">
       <c r="A14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="12.75" customHeight="1">
+    <row r="15" spans="1:6" ht="12.75" customHeight="1">
       <c r="A15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="12.75" customHeight="1">
+    <row r="16" spans="1:6" ht="12.75" customHeight="1">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -3042,7 +3076,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3069,25 +3103,25 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3098,10 +3132,10 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>40213</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>41139</v>
       </c>
       <c r="E5" t="s">
@@ -3121,10 +3155,10 @@
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>40224</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>41143</v>
       </c>
       <c r="E6" t="s">
@@ -3144,10 +3178,10 @@
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>40244</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>41200</v>
       </c>
       <c r="E7" t="s">
@@ -3167,10 +3201,10 @@
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>40249</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>41220</v>
       </c>
       <c r="E8" t="s">
@@ -3190,10 +3224,10 @@
       <c r="B9">
         <v>5</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>40266</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>41197</v>
       </c>
       <c r="E9" t="s">
@@ -3213,10 +3247,10 @@
       <c r="B10">
         <v>5</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>40273</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>41233</v>
       </c>
       <c r="E10" t="s">
@@ -3236,10 +3270,10 @@
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>40278</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>41242</v>
       </c>
       <c r="E11" t="s">
@@ -3259,10 +3293,10 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>40290</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <v>41204</v>
       </c>
       <c r="E12" t="s">
@@ -3282,10 +3316,10 @@
       <c r="B13">
         <v>4</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <v>40301</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <v>41219</v>
       </c>
       <c r="E13" t="s">
@@ -3299,72 +3333,72 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A14" s="12">
+      <c r="A14" s="11">
         <v>8</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="11">
         <v>2</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="12">
         <v>40290</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="12">
         <v>41260</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="11">
         <v>4351.99</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="11">
         <v>288.42</v>
       </c>
     </row>
     <row r="18" spans="3:3" ht="12.75" customHeight="1">
-      <c r="C18" s="11"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" spans="3:3" ht="12.75" customHeight="1">
-      <c r="C19" s="11"/>
+      <c r="C19" s="10"/>
     </row>
     <row r="20" spans="3:3" ht="12.75" customHeight="1">
-      <c r="C20" s="11"/>
+      <c r="C20" s="10"/>
     </row>
     <row r="21" spans="3:3" ht="12.75" customHeight="1">
-      <c r="C21" s="11"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" spans="3:3" ht="12.75" customHeight="1">
-      <c r="C22" s="11"/>
+      <c r="C22" s="10"/>
     </row>
     <row r="23" spans="3:3" ht="12.75" customHeight="1">
-      <c r="C23" s="11"/>
+      <c r="C23" s="10"/>
     </row>
     <row r="24" spans="3:3" ht="12.75" customHeight="1">
-      <c r="C24" s="11"/>
+      <c r="C24" s="10"/>
     </row>
     <row r="25" spans="3:3" ht="12.75" customHeight="1">
-      <c r="C25" s="11"/>
+      <c r="C25" s="10"/>
     </row>
     <row r="26" spans="3:3" ht="12.75" customHeight="1">
-      <c r="C26" s="11"/>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" spans="3:3" ht="12.75" customHeight="1">
-      <c r="C27" s="11"/>
+      <c r="C27" s="10"/>
     </row>
     <row r="28" spans="3:3" ht="12.75" customHeight="1">
-      <c r="C28" s="11"/>
+      <c r="C28" s="10"/>
     </row>
     <row r="29" spans="3:3" ht="12.75" customHeight="1">
-      <c r="C29" s="11"/>
+      <c r="C29" s="10"/>
     </row>
     <row r="30" spans="3:3" ht="12.75" customHeight="1">
-      <c r="C30" s="11"/>
+      <c r="C30" s="10"/>
     </row>
     <row r="31" spans="3:3" ht="12.75" customHeight="1">
-      <c r="C31" s="11"/>
+      <c r="C31" s="10"/>
     </row>
     <row r="32" spans="3:3" ht="12.75" customHeight="1">
-      <c r="C32" s="11"/>
+      <c r="C32" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.78739999999999999" right="0.78739999999999999" top="1.2792000000000001" bottom="1.2792000000000001" header="0.9839" footer="0.9839"/>
@@ -3374,7 +3408,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3393,50 +3427,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11">
         <v>2.95</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="14" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3447,7 +3481,7 @@
       <c r="B4">
         <v>50</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <v>1.25</v>
       </c>
     </row>
@@ -3458,7 +3492,7 @@
       <c r="B5">
         <v>120</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <v>3.4</v>
       </c>
     </row>
@@ -3469,23 +3503,23 @@
       <c r="B6">
         <v>200</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="15">
         <v>0.75</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="11">
         <v>45</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="16">
         <v>8.5</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.78739999999999999" right="0.78739999999999999" top="1.2792000000000001" bottom="1.2792000000000001" header="0.9839" footer="0.9839"/>

</xml_diff>